<commit_message>
#69 Layer.copyRect, operateRect, stretchCopy, operateStretch, affineCopy, operateAffine の src に Bitmap クラスも指定可能にした。 バージョン番号を上げた。
</commit_message>
<xml_diff>
--- a/msg/text/Messages.xlsx
+++ b/msg/text/Messages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19200" windowHeight="12090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TJS2" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="1179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="1185">
   <si>
     <t>TJSInternalError</t>
   </si>
@@ -4613,6 +4613,39 @@
   </si>
   <si>
     <t>TVPCannotShowModalSingleWindow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TVPSpecifyLayerOrBitmap</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Layer クラスか Bitmap クラスのオブジェクトを指定してください</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Specify Layer or Bitmap class object</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TVPCannotAcceptModeAuto</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cannot accept omAuto mode</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>この操作で mode に omAuto を指定することは出来ません</t>
+    <rPh sb="2" eb="4">
+      <t>ソウサ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>デキ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -5866,10 +5899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -6389,547 +6422,541 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>241</v>
+        <v>1179</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>336</v>
+        <v>1180</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>927</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>242</v>
+        <v>1182</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>337</v>
+        <v>1184</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>928</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A63" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A69" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A76" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A82" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A83" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>724</v>
+        <v>288</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>723</v>
+        <v>377</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A91" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>379</v>
+        <v>970</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A92" s="1" t="s">
-        <v>677</v>
+        <v>724</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>649</v>
+        <v>723</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
-        <v>685</v>
+        <v>290</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>647</v>
+        <v>380</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>482</v>
+        <v>379</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
-        <v>686</v>
+        <v>677</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>482</v>
+        <v>972</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A95" s="1" t="s">
-        <v>678</v>
+        <v>685</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>643</v>
+        <v>647</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>480</v>
+        <v>469</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>482</v>
@@ -6937,13 +6964,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A96" s="1" t="s">
-        <v>679</v>
+        <v>686</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>644</v>
+        <v>648</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>482</v>
@@ -6951,13 +6978,13 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A97" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>482</v>
@@ -6965,13 +6992,13 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>482</v>
@@ -6979,13 +7006,13 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>481</v>
+        <v>645</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>482</v>
@@ -6993,13 +7020,13 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>681</v>
+        <v>687</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>472</v>
+        <v>646</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>482</v>
@@ -7007,13 +7034,13 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>473</v>
+        <v>481</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>482</v>
@@ -7021,13 +7048,13 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A102" s="1" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>482</v>
@@ -7035,13 +7062,13 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A103" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>482</v>
@@ -7049,13 +7076,13 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A104" s="1" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>650</v>
+        <v>479</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>482</v>
@@ -7063,13 +7090,13 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A105" s="1" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>482</v>
@@ -7077,510 +7104,538 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A106" s="1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>483</v>
+        <v>650</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A107" s="1" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>484</v>
+        <v>476</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A108" s="1" t="s">
-        <v>531</v>
+        <v>691</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>532</v>
+        <v>483</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A109" s="1" t="s">
-        <v>725</v>
+        <v>692</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A110" s="1" t="s">
-        <v>726</v>
+        <v>531</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>651</v>
+        <v>487</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>489</v>
+        <v>532</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A111" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>722</v>
+        <v>488</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A112" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>491</v>
+        <v>651</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A113" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>492</v>
+        <v>722</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A114" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A116" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A117" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A118" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>714</v>
+        <v>495</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A119" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>715</v>
+        <v>496</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A120" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>499</v>
+        <v>714</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A121" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>500</v>
+        <v>715</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A122" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>716</v>
+        <v>499</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>717</v>
+        <v>500</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>507</v>
+        <v>719</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>510</v>
+        <v>721</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>712</v>
+        <v>512</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>711</v>
+        <v>513</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>518</v>
+        <v>710</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>519</v>
+        <v>709</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>707</v>
+        <v>520</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>708</v>
+        <v>521</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A152" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A153" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B153" s="1" t="s">
         <v>700</v>
       </c>
-      <c r="C151" s="1" t="s">
+      <c r="C153" s="1" t="s">
         <v>530</v>
       </c>
     </row>
@@ -7599,7 +7654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A194" sqref="A194"/>
     </sheetView>
   </sheetViews>

</xml_diff>